<commit_message>
1 task step 1 database (#3)
* 230124

* 230125

* 230125

* rdb import 완료
</commit_message>
<xml_diff>
--- a/data/Variable_info.xlsx
+++ b/data/Variable_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\user\Github\AIB15\Projects\Kor-DEEPression\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CD1570-0B54-4AA4-9656-7B4F32097C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD347BB-74F8-4F3D-A70B-291042B14D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28860" yWindow="5370" windowWidth="16005" windowHeight="15135" xr2:uid="{EE446920-0EED-43F1-9778-DFA11599149A}"/>
+    <workbookView xWindow="28905" yWindow="6315" windowWidth="16005" windowHeight="15135" xr2:uid="{EE446920-0EED-43F1-9778-DFA11599149A}"/>
   </bookViews>
   <sheets>
     <sheet name="변수 정리" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="164">
   <si>
     <t>변수명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -684,6 +684,30 @@
   </si>
   <si>
     <t>우울증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서당,한학/무학/초등학교/중등/고등/2~3년제/4년제/대학원/99</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1~2 : 유배우자 / 3~4 : 사별 이혼 / 88 : 미혼 /99</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 : 취업자 / 2 : 실업자,비경제활동인구 /9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1~6, 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최근 1년 동안의 음주(술) 경험에 대한 질문입니다. 술을 얼마나 자주 마십니까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최근 1년 동안의 음주(술) 경험에 대한 질문입니다. 한번에 술을 얼마나 마십니까?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -749,7 +773,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,22 +783,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1091,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812D4A18-51A8-4F05-99E1-61A71D2C29A7}">
-  <dimension ref="B2:G37"/>
+  <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1109,7 +1127,7 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1126,51 +1144,51 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
-      <c r="C4" s="8" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>75</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
         <v>71</v>
       </c>
@@ -1184,8 +1202,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
         <v>72</v>
       </c>
@@ -1199,70 +1217,73 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="4" t="s">
         <v>152</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="6" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="8" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>99</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1279,14 +1300,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="8" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1296,7 +1317,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1313,51 +1334,60 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="8" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>99</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="4" t="s">
         <v>85</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="8" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>9</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="4" t="s">
         <v>88</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1367,14 +1397,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C21" s="8" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1384,14 +1417,17 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C22" s="8" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>9</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -1401,14 +1437,14 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C23" s="5" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1418,14 +1454,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="8" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="3" t="s">
         <v>88</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -1435,14 +1471,17 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="8" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>9</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="4" t="s">
         <v>120</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1452,14 +1491,14 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C26" s="8" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -1469,34 +1508,34 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C29" s="8" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -1506,62 +1545,71 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C30" s="8" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>78</v>
+      <c r="E30" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>131</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C31" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>9</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="4" t="s">
         <v>133</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>134</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C32" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C32" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="4" t="s">
         <v>145</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C33" s="8" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>9</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="4" t="s">
         <v>77</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -1571,7 +1619,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>157</v>
       </c>
@@ -1588,7 +1636,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1602,14 +1650,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C37" s="1" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
@@ -1667,7 +1715,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1681,7 +1729,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>